<commit_message>
Creating big table, containing every value of other small tables
</commit_message>
<xml_diff>
--- a/data/raw/2014/Acinetobacter/acinetobacter-resistance-combinations-2014.xlsx
+++ b/data/raw/2014/Acinetobacter/acinetobacter-resistance-combinations-2014.xlsx
@@ -139,6 +139,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -147,12 +153,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFffffff"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -306,7 +306,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -318,37 +318,31 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -360,26 +354,26 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -692,11 +686,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="29" width="47.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="30" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="31" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="32" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="27" width="47.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="28" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="29" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="30" width="10.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.625" customFormat="1" s="1">
@@ -715,7 +709,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -739,160 +733,160 @@
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="8">
         <v>1511</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="9">
         <v>38.6</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="21"/>
+      <c r="E6" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="21">
         <f>B8+B9+B10</f>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <f>C8+C9+C10</f>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="8">
         <v>98</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="9">
         <v>2.5</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="8">
         <v>48</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="9">
         <v>1.2</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="8">
         <v>22</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="9">
         <v>0.6</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="21"/>
+      <c r="E10" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="21"/>
+      <c r="E11" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="21">
         <f>B13+B14+B15</f>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="22">
         <f>C13+C14+C15</f>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="21"/>
+      <c r="E12" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="8">
         <v>201</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="9">
         <v>5.1</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="8">
         <v>149</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="9">
         <v>3.8</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="21"/>
+      <c r="E14" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="8">
         <v>11</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="9">
         <v>0.3</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="21"/>
+      <c r="E16" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="8">
         <v>1870</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="9">
         <v>47.8</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="21"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="E17" s="19"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -900,7 +894,7 @@
       <c r="E18" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="8"/>
@@ -909,7 +903,7 @@
       <c r="E19" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="8"/>

</xml_diff>